<commit_message>
Project 1 code till Sep 26th
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/excels/MasterTestData.xlsx
+++ b/target/test-classes/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\012LivetechWS\HybridFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C3564E-CB04-4220-BFC6-4CE7D2939E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B120EDA-3E7D-4BDF-AB1A-6D1CA4E10510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A176B97-7D08-43CF-852F-819A98689553}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>